<commit_message>
finished the basic functions!!!
</commit_message>
<xml_diff>
--- a/data/life.xlsx
+++ b/data/life.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>id</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>39.986913,116.3036799</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>001.png</t>
+  </si>
+  <si>
+    <t>002.png</t>
   </si>
 </sst>
 </file>
@@ -943,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +967,7 @@
     <col min="12" max="12" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1001,8 +1010,11 @@
       <c r="N1" t="s">
         <v>11</v>
       </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1024,8 +1036,11 @@
       <c r="N2" t="s">
         <v>15</v>
       </c>
+      <c r="O2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1050,8 +1065,11 @@
       <c r="N3" t="s">
         <v>25</v>
       </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
this work is currently finished. Remining work will be focused on adding more data and optimizingg the visualization strategy
</commit_message>
<xml_diff>
--- a/data/life.xlsx
+++ b/data/life.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -63,15 +63,6 @@
     <t>2007,8,2</t>
   </si>
   <si>
-    <t>Got the offer form the top ranked university, best day ever in my life!</t>
-  </si>
-  <si>
-    <t>34.263673, 108.185418</t>
-  </si>
-  <si>
-    <t>Begin my trip to Beijing</t>
-  </si>
-  <si>
     <t>2007,9,2</t>
   </si>
   <si>
@@ -87,27 +78,9 @@
     <t>classname</t>
   </si>
   <si>
-    <t>No comment</t>
-  </si>
-  <si>
-    <t>Begin my first programming class</t>
-  </si>
-  <si>
-    <t>2007,10,4</t>
-  </si>
-  <si>
     <t>34.2762584,108.958004,39.894884,116.318922</t>
   </si>
   <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
     <t>39.986913,116.3036799</t>
   </si>
   <si>
@@ -118,6 +91,321 @@
   </si>
   <si>
     <t>002.png</t>
+  </si>
+  <si>
+    <t>eventType</t>
+  </si>
+  <si>
+    <t>2007,8,1</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>34.2637922,108.1898902</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>intro.png</t>
+  </si>
+  <si>
+    <t>34.264422,108.0758482</t>
+  </si>
+  <si>
+    <t>Hi, my name is Hu Shao. I build up this webpage to record and display some interesting footprints of my daily life since 2007 (the year when I became a freshman). Each event are displayed on the timeline, map the the information panel according to its time order. The three things are connected. When you click one of them, the others will be highlighted. The current location is my hometown where I grow up, and where my story begins</t>
+  </si>
+  <si>
+    <t>entertainment</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>My trip to Beijing</t>
+  </si>
+  <si>
+    <t>My first programming class</t>
+  </si>
+  <si>
+    <t>The first programming course in mylife, which is c language</t>
+  </si>
+  <si>
+    <t>Got the offer form the top ranked university, best day ever!</t>
+  </si>
+  <si>
+    <t>003.png</t>
+  </si>
+  <si>
+    <t>2014 New Year Celebration</t>
+  </si>
+  <si>
+    <t>2014,1,2</t>
+  </si>
+  <si>
+    <t>Last new year celebration with my dear friends in Peking Univ. A wonderful time</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>2014-year-cel.png</t>
+  </si>
+  <si>
+    <t>39.9893137,116.3032347</t>
+  </si>
+  <si>
+    <t>Back to my hometown</t>
+  </si>
+  <si>
+    <t>2008,2,2</t>
+  </si>
+  <si>
+    <t>Return back to my hometown for the traditonal Chinese new year. A tough semestar. But I survived.</t>
+  </si>
+  <si>
+    <t>Visiting the military museum of Beijing</t>
+  </si>
+  <si>
+    <t>2008,1,31</t>
+  </si>
+  <si>
+    <t>005.png</t>
+  </si>
+  <si>
+    <t>After the semester, I took a visit to the China's biggest military museum in Beijing</t>
+  </si>
+  <si>
+    <t>006.png</t>
+  </si>
+  <si>
+    <t>34.2561421,108.1863839</t>
+  </si>
+  <si>
+    <t>39.9074641,116.322745</t>
+  </si>
+  <si>
+    <t>2007,10,3</t>
+  </si>
+  <si>
+    <t>007.png</t>
+  </si>
+  <si>
+    <t>The Xiangshan hiking</t>
+  </si>
+  <si>
+    <t>2007,9,4</t>
+  </si>
+  <si>
+    <t>A hiking trip with my classmates to Xiangshan, which is close to my Univ. Look how slim at those days!</t>
+  </si>
+  <si>
+    <t>Beijing's Olympic Games</t>
+  </si>
+  <si>
+    <t>2008,8,8</t>
+  </si>
+  <si>
+    <t>2008,9,17</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>008.png</t>
+  </si>
+  <si>
+    <t>39.9928671,116.394394</t>
+  </si>
+  <si>
+    <t>The Olympic games Was held in Beijing, China. A  historic event. I was luckily been selected as the volunteer for the following Paralympic Games.</t>
+  </si>
+  <si>
+    <t>Hike and BBQ</t>
+  </si>
+  <si>
+    <t>2008,11,4</t>
+  </si>
+  <si>
+    <t>A hiking and barbecue with my classmates to celebrate the coming winter</t>
+  </si>
+  <si>
+    <t>009.png</t>
+  </si>
+  <si>
+    <t>40.3516526,115.8216491</t>
+  </si>
+  <si>
+    <t>2009 New Year Celebration</t>
+  </si>
+  <si>
+    <t>2008,12,27</t>
+  </si>
+  <si>
+    <t>010.png</t>
+  </si>
+  <si>
+    <t>39.9936661,116.296406,39.9921801,116.184539</t>
+  </si>
+  <si>
+    <t>My field trip in HeNan Province - 1</t>
+  </si>
+  <si>
+    <t>2009,7,6</t>
+  </si>
+  <si>
+    <t>2009,7,14</t>
+  </si>
+  <si>
+    <t>This is a field investigation in HeNan Province, China. We investigated the tobacco growing situtation in some cities of this province. Then, by using these data and remote sensing imagery, we can evaluate the future tobacco output of the whole province.</t>
+  </si>
+  <si>
+    <t>2010,8,1</t>
+  </si>
+  <si>
+    <t>2010,8,7</t>
+  </si>
+  <si>
+    <t>39.894884,116.318922,35.2875244,113.960183,34.8292374,114.359643,33.5827674,114.654685,34.0200474,113.90595,34.6806604,113.554193</t>
+  </si>
+  <si>
+    <t>39.894884,116.318922,34.7908924,111.178029,34.6010584,112.53406,33.6974784,113.178207,32.9685615,112.576239,33.0214615,113.968299,32.1647855,114.02625</t>
+  </si>
+  <si>
+    <t>This is a following up investigation of last years trip</t>
+  </si>
+  <si>
+    <t>011.png</t>
+  </si>
+  <si>
+    <t>My field trip in HeNan Province - 2</t>
+  </si>
+  <si>
+    <t>The celebration party of our departmant to celebrate the new year. We prepared a show named as 'Dancing of Monsters'</t>
+  </si>
+  <si>
+    <t>014.png</t>
+  </si>
+  <si>
+    <t>Girl's day celebration</t>
+  </si>
+  <si>
+    <t>2010,3,7</t>
+  </si>
+  <si>
+    <t>Gethering together with my classmates and celebrate the 'Girl's Day' - which is a very pupolar festival in universities of China, especially in those which have more boys than girls.</t>
+  </si>
+  <si>
+    <t>39.9919011,116.304377</t>
+  </si>
+  <si>
+    <t>Hiking</t>
+  </si>
+  <si>
+    <t>2010,3,16</t>
+  </si>
+  <si>
+    <t>015.png</t>
+  </si>
+  <si>
+    <t>39.8750305,116.376886</t>
+  </si>
+  <si>
+    <t>Hiking in the early spring, In Taoranting Park, Beijing</t>
+  </si>
+  <si>
+    <t>016.png</t>
+  </si>
+  <si>
+    <t>2010,5,3</t>
+  </si>
+  <si>
+    <t>Drift</t>
+  </si>
+  <si>
+    <t>Drift in Shidu, Beijing</t>
+  </si>
+  <si>
+    <t>2010,5,5</t>
+  </si>
+  <si>
+    <t>39.6311811,115.571053,39.6333411,115.578071,39.6368971,115.5843481,39.6328941,115.5875604,39.630489,115.5869112</t>
+  </si>
+  <si>
+    <t>After-graduation trip</t>
+  </si>
+  <si>
+    <t>2011,6,11</t>
+  </si>
+  <si>
+    <t>2011,6,15</t>
+  </si>
+  <si>
+    <t>Graduation</t>
+  </si>
+  <si>
+    <t>2011,6,9</t>
+  </si>
+  <si>
+    <t>In 2011's summer, I graduated from Peking University, got the Bachelor Degree of Geographic Information Science</t>
+  </si>
+  <si>
+    <t>017.png</t>
+  </si>
+  <si>
+    <t>39.9906694,116.3037346</t>
+  </si>
+  <si>
+    <t>018.png</t>
+  </si>
+  <si>
+    <t>After the graduation, We arranged a 5 days' trip in HuNan Province. Three major scenic areas were visited.</t>
+  </si>
+  <si>
+    <t>29.3155337,110.426965</t>
+  </si>
+  <si>
+    <t>39.895466, 116.315096,29.3155337,110.426965,27.951181, 109.600950,28.194523, 113.011277</t>
+  </si>
+  <si>
+    <t>2011,6,12</t>
+  </si>
+  <si>
+    <t>Trip - stop 1</t>
+  </si>
+  <si>
+    <t>The first stop of  the after graduate trip - Zhangjiajie natonal forest park</t>
+  </si>
+  <si>
+    <t>019.png</t>
+  </si>
+  <si>
+    <t>Trip - stop 2</t>
+  </si>
+  <si>
+    <t>Trip - stop 3</t>
+  </si>
+  <si>
+    <t>The second stop of  the after graduate trip - Fenghuang (Phoenix) ancient town</t>
+  </si>
+  <si>
+    <t>The third stop of  the after graduate trip - Changsha City (the capital of HuNan Province)</t>
+  </si>
+  <si>
+    <t>27.951181, 109.600950</t>
+  </si>
+  <si>
+    <t>28.194523, 113.011277</t>
+  </si>
+  <si>
+    <t>2011,6,14</t>
+  </si>
+  <si>
+    <t>020.png</t>
+  </si>
+  <si>
+    <t>021.png</t>
   </si>
 </sst>
 </file>
@@ -601,8 +889,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -952,22 +1243,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection sqref="A1:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="68" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="68" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="64.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,113 +1277,2222 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>18</v>
       </c>
-      <c r="E3" t="b">
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="b">
+      <c r="H19" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" t="b">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" t="s">
-        <v>29</v>
+      <c r="F20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="107" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="108" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="110" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="111" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="112" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="113" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="114" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H115" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H116" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="117" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H117" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="119" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="122" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="123" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="124" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="125" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="126" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="127" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H128" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H129" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H130" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H131" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H132" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H133" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H134" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H135" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H136" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="137" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H137" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="138" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="139" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H139" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="140" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="141" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H141" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H142" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="145" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="146" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="147" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="148" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="149" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="150" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="151" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="152" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="153" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="154" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="155" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H155" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="156" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H156" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="157" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H157" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="158" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H158" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="159" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H159" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="160" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H160" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="161" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H161" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="162" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H162" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="163" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H163" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="164" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H164" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="165" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H165" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="166" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H166" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="167" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H167" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H168" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="169" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H169" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="170" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H170" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="171" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H171" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="172" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H172" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="173" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H173" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="174" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H174" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="175" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H175" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="176" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H176" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="177" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H177" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="178" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H178" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="179" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H179" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="180" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H180" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="181" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H181" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="182" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H182" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="183" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H183" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="184" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H184" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="185" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H185" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="186" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H186" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="187" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H187" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="188" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H188" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="189" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H189" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="190" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H190" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="191" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H191" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="192" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H192" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="193" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H193" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="194" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H194" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="195" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H195" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="196" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H196" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="197" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H197" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="198" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H198" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="199" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H199" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="200" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H200" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="201" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H201" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="202" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H202" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="203" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H203" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="204" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H204" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="205" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H205" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="206" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H206" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="207" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H207" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="208" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H208" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="209" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H209" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="210" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H210" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="211" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H211" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="212" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H212" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="213" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H213" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="214" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H214" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="215" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H215" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="216" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H216" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="217" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H217" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="218" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H218" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="219" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H219" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="220" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H220" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="221" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H221" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="222" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H222" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="223" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H223" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="224" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H224" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="225" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H225" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="226" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H226" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="227" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H227" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="228" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H228" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="229" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H229" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="230" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H230" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="231" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H231" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="232" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H232" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="233" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H233" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="234" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H234" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="235" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H235" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="236" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H236" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="237" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H237" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="238" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H238" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="239" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H239" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="240" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H240" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="241" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H241" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="242" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H242" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="243" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H243" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="244" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H244" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="245" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H245" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="246" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H246" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="247" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H247" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="248" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H248" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="249" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H249" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="250" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H250" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="251" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H251" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="252" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H252" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="253" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H253" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="254" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H254" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="255" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H255" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="256" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H256" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="257" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H257" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="258" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H258" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="259" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H259" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="260" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H260" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="261" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H261" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="262" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H262" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="263" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H263" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="264" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H264" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="265" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H265" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="266" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H266" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="267" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H267" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="268" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H268" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="269" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H269" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="270" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H270" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="271" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H271" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="272" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H272" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="273" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H273" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="274" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H274" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="275" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H275" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="276" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H276" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="277" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H277" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="278" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H278" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="279" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H279" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="280" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H280" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="281" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H281" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="282" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H282" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="283" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H283" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="284" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H284" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="285" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H285" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="286" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H286" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="287" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H287" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="288" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H288" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="289" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H289" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="290" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H290" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="291" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H291" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="292" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H292" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="293" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H293" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="294" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H294" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="295" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H295" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="296" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H296" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="297" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H297" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="298" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H298" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="299" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H299" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="300" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H300" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="301" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H301" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="302" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H302" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="303" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H303" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="304" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H304" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="305" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H305" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="306" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H306" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="307" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H307" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="308" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H308" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="309" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H309" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="310" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H310" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="311" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H311" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="312" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H312" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="313" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H313" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="314" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H314" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="315" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H315" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="316" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H316" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="317" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H317" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="318" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H318" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="319" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H319" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="320" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H320" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="321" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H321" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="322" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H322" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="323" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H323" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="324" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H324" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="325" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H325" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="326" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H326" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="327" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H327" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="328" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H328" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="329" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H329" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="330" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H330" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="331" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H331" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="332" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H332" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="333" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H333" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="334" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H334" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="335" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H335" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="336" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H336" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="337" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H337" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="338" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H338" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="339" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H339" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="340" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H340" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="341" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H341" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="342" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H342" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="343" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H343" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="344" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H344" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="345" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H345" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="346" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H346" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="347" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H347" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="348" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H348" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="349" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H349" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="350" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H350" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="351" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H351" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="352" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H352" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="353" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H353" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="354" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H354" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="355" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H355" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="356" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H356" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="357" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H357" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="358" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H358" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="359" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H359" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="360" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H360" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="361" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H361" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="362" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H362" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="363" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H363" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="364" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H364" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="365" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H365" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="366" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H366" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="367" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H367" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="368" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H368" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="369" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H369" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="370" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H370" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="371" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H371" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="372" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H372" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="373" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H373" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="374" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H374" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="375" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H375" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="376" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H376" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="377" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H377" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="378" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H378" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="379" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H379" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="380" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H380" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="381" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H381" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="382" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H382" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="383" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H383" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="384" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H384" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="385" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H385" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="386" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H386" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="387" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H387" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="388" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H388" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="389" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H389" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="390" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H390" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="391" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H391" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="392" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H392" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="393" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H393" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="394" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H394" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="395" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H395" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="396" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H396" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="397" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H397" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="398" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H398" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="399" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H399" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="400" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H400" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="401" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H401" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="402" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H402" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="403" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H403" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="404" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H404" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="405" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H405" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="406" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H406" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="407" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H407" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="408" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H408" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="409" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H409" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="410" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H410" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="411" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H411" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="412" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H412" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="413" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H413" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="414" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H414" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="415" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H415" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="416" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H416" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>